<commit_message>
Fixed strata percentile and height array (Neighborhood). Added record promotion in simulationRun.
</commit_message>
<xml_diff>
--- a/WebContent/data/fg.xlsx
+++ b/WebContent/data/fg.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="27">
   <si>
     <t>Name</t>
   </si>
@@ -95,6 +95,9 @@
   </si>
   <si>
     <t>Sapling</t>
+  </si>
+  <si>
+    <t>Emergent</t>
   </si>
 </sst>
 </file>
@@ -492,10 +495,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -521,10 +524,10 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>26</v>
       </c>
       <c r="C2">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -532,10 +535,10 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="C3">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -543,10 +546,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C4">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -554,21 +557,21 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C5">
-        <v>0.4</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>25</v>
+        <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="C6">
-        <v>0.1</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -576,10 +579,10 @@
         <v>25</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="C7">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -587,10 +590,10 @@
         <v>25</v>
       </c>
       <c r="B8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C8">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -598,9 +601,20 @@
         <v>25</v>
       </c>
       <c r="B9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" t="s">
         <v>17</v>
       </c>
-      <c r="C9">
+      <c r="C10">
         <v>0.4</v>
       </c>
     </row>
@@ -612,10 +626,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -643,7 +657,7 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>26</v>
       </c>
       <c r="C2" t="s">
         <v>19</v>
@@ -654,18 +668,18 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="C3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15.75">
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>16</v>
+      <c r="B4" t="s">
+        <v>15</v>
       </c>
       <c r="C4" t="s">
         <v>19</v>
@@ -676,18 +690,18 @@
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C5" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" ht="15.75">
       <c r="A6" t="s">
-        <v>25</v>
-      </c>
-      <c r="B6" t="s">
-        <v>4</v>
+        <v>3</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>17</v>
       </c>
       <c r="C6" t="s">
         <v>19</v>
@@ -698,18 +712,18 @@
         <v>25</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="C7" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="15.75">
+    <row r="8" spans="1:3">
       <c r="A8" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>16</v>
+      <c r="B8" t="s">
+        <v>15</v>
       </c>
       <c r="C8" t="s">
         <v>19</v>
@@ -720,9 +734,20 @@
         <v>25</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="15.75">
+      <c r="A10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C10" t="s">
         <v>19</v>
       </c>
     </row>
@@ -734,10 +759,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G49"/>
+  <dimension ref="A1:G55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C45" sqref="C45"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -775,7 +800,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>4</v>
+        <v>26</v>
       </c>
       <c r="C2" t="s">
         <v>11</v>
@@ -798,7 +823,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>4</v>
+        <v>26</v>
       </c>
       <c r="C3" t="s">
         <v>11</v>
@@ -821,7 +846,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>4</v>
+        <v>26</v>
       </c>
       <c r="C4" t="s">
         <v>11</v>
@@ -844,7 +869,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>4</v>
+        <v>26</v>
       </c>
       <c r="C5" t="s">
         <v>12</v>
@@ -867,7 +892,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>4</v>
+        <v>26</v>
       </c>
       <c r="C6" t="s">
         <v>12</v>
@@ -890,7 +915,7 @@
         <v>3</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>4</v>
+        <v>26</v>
       </c>
       <c r="C7" t="s">
         <v>12</v>
@@ -908,12 +933,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="15.75">
+    <row r="8" spans="1:7">
       <c r="A8" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>15</v>
+      <c r="B8" s="2" t="s">
+        <v>4</v>
       </c>
       <c r="C8" t="s">
         <v>11</v>
@@ -922,21 +947,21 @@
         <v>12</v>
       </c>
       <c r="E8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="15.75">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
       <c r="A9" t="s">
         <v>3</v>
       </c>
-      <c r="B9" s="3" t="s">
-        <v>15</v>
+      <c r="B9" s="2" t="s">
+        <v>4</v>
       </c>
       <c r="C9" t="s">
         <v>11</v>
@@ -945,21 +970,21 @@
         <v>13</v>
       </c>
       <c r="E9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G9">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="15.75">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
       <c r="A10" t="s">
         <v>3</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>15</v>
+      <c r="B10" s="2" t="s">
+        <v>4</v>
       </c>
       <c r="C10" t="s">
         <v>11</v>
@@ -968,21 +993,21 @@
         <v>14</v>
       </c>
       <c r="E10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G10">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="15.75">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
       <c r="A11" t="s">
         <v>3</v>
       </c>
-      <c r="B11" s="3" t="s">
-        <v>15</v>
+      <c r="B11" s="2" t="s">
+        <v>4</v>
       </c>
       <c r="C11" t="s">
         <v>12</v>
@@ -991,21 +1016,21 @@
         <v>11</v>
       </c>
       <c r="E11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G11">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="15.75">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
       <c r="A12" t="s">
         <v>3</v>
       </c>
-      <c r="B12" s="3" t="s">
-        <v>15</v>
+      <c r="B12" s="2" t="s">
+        <v>4</v>
       </c>
       <c r="C12" t="s">
         <v>12</v>
@@ -1014,21 +1039,21 @@
         <v>13</v>
       </c>
       <c r="E12">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F12">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G12">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="15.75">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
       <c r="A13" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="3" t="s">
-        <v>15</v>
+      <c r="B13" s="2" t="s">
+        <v>4</v>
       </c>
       <c r="C13" t="s">
         <v>12</v>
@@ -1037,21 +1062,21 @@
         <v>14</v>
       </c>
       <c r="E13">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F13">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G13">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="15.75">
       <c r="A14" t="s">
         <v>3</v>
       </c>
-      <c r="B14" s="4" t="s">
-        <v>16</v>
+      <c r="B14" s="3" t="s">
+        <v>15</v>
       </c>
       <c r="C14" t="s">
         <v>11</v>
@@ -1060,21 +1085,21 @@
         <v>12</v>
       </c>
       <c r="E14">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F14">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G14">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="15.75">
       <c r="A15" t="s">
         <v>3</v>
       </c>
-      <c r="B15" s="4" t="s">
-        <v>16</v>
+      <c r="B15" s="3" t="s">
+        <v>15</v>
       </c>
       <c r="C15" t="s">
         <v>11</v>
@@ -1083,21 +1108,21 @@
         <v>13</v>
       </c>
       <c r="E15">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F15">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G15">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="15.75">
       <c r="A16" t="s">
         <v>3</v>
       </c>
-      <c r="B16" s="4" t="s">
-        <v>16</v>
+      <c r="B16" s="3" t="s">
+        <v>15</v>
       </c>
       <c r="C16" t="s">
         <v>11</v>
@@ -1106,21 +1131,21 @@
         <v>14</v>
       </c>
       <c r="E16">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F16">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G16">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="15.75">
       <c r="A17" t="s">
         <v>3</v>
       </c>
-      <c r="B17" s="4" t="s">
-        <v>16</v>
+      <c r="B17" s="3" t="s">
+        <v>15</v>
       </c>
       <c r="C17" t="s">
         <v>12</v>
@@ -1129,21 +1154,21 @@
         <v>11</v>
       </c>
       <c r="E17">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F17">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G17">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="15.75">
       <c r="A18" t="s">
         <v>3</v>
       </c>
-      <c r="B18" s="4" t="s">
-        <v>16</v>
+      <c r="B18" s="3" t="s">
+        <v>15</v>
       </c>
       <c r="C18" t="s">
         <v>12</v>
@@ -1152,21 +1177,21 @@
         <v>13</v>
       </c>
       <c r="E18">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F18">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G18">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="15.75">
       <c r="A19" t="s">
         <v>3</v>
       </c>
-      <c r="B19" s="4" t="s">
-        <v>16</v>
+      <c r="B19" s="3" t="s">
+        <v>15</v>
       </c>
       <c r="C19" t="s">
         <v>12</v>
@@ -1175,13 +1200,13 @@
         <v>14</v>
       </c>
       <c r="E19">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F19">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G19">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="15.75">
@@ -1189,7 +1214,7 @@
         <v>3</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C20" t="s">
         <v>11</v>
@@ -1198,13 +1223,13 @@
         <v>12</v>
       </c>
       <c r="E20">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F20">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G20">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="15.75">
@@ -1212,7 +1237,7 @@
         <v>3</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C21" t="s">
         <v>11</v>
@@ -1221,13 +1246,13 @@
         <v>13</v>
       </c>
       <c r="E21">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F21">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G21">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="15.75">
@@ -1235,7 +1260,7 @@
         <v>3</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C22" t="s">
         <v>11</v>
@@ -1244,13 +1269,13 @@
         <v>14</v>
       </c>
       <c r="E22">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F22">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G22">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="15.75">
@@ -1258,7 +1283,7 @@
         <v>3</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C23" t="s">
         <v>12</v>
@@ -1267,13 +1292,13 @@
         <v>11</v>
       </c>
       <c r="E23">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F23">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G23">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="15.75">
@@ -1281,7 +1306,7 @@
         <v>3</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C24" t="s">
         <v>12</v>
@@ -1290,13 +1315,13 @@
         <v>13</v>
       </c>
       <c r="E24">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F24">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G24">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="15.75">
@@ -1304,7 +1329,7 @@
         <v>3</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C25" t="s">
         <v>12</v>
@@ -1313,21 +1338,21 @@
         <v>14</v>
       </c>
       <c r="E25">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F25">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G25">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="15.75">
       <c r="A26" t="s">
-        <v>25</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>17</v>
       </c>
       <c r="C26" t="s">
         <v>11</v>
@@ -1336,21 +1361,21 @@
         <v>12</v>
       </c>
       <c r="E26">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F26">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G26">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="15.75">
       <c r="A27" t="s">
-        <v>25</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>17</v>
       </c>
       <c r="C27" t="s">
         <v>11</v>
@@ -1359,21 +1384,21 @@
         <v>13</v>
       </c>
       <c r="E27">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F27">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G27">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="15.75">
       <c r="A28" t="s">
-        <v>25</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>17</v>
       </c>
       <c r="C28" t="s">
         <v>11</v>
@@ -1382,21 +1407,21 @@
         <v>14</v>
       </c>
       <c r="E28">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F28">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G28">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="15.75">
       <c r="A29" t="s">
-        <v>25</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>17</v>
       </c>
       <c r="C29" t="s">
         <v>12</v>
@@ -1405,21 +1430,21 @@
         <v>11</v>
       </c>
       <c r="E29">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F29">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G29">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="15.75">
       <c r="A30" t="s">
-        <v>25</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>17</v>
       </c>
       <c r="C30" t="s">
         <v>12</v>
@@ -1428,21 +1453,21 @@
         <v>13</v>
       </c>
       <c r="E30">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F30">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G30">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="15.75">
       <c r="A31" t="s">
-        <v>25</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>17</v>
       </c>
       <c r="C31" t="s">
         <v>12</v>
@@ -1451,21 +1476,21 @@
         <v>14</v>
       </c>
       <c r="E31">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F31">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G31">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" ht="15.75">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7">
       <c r="A32" t="s">
         <v>25</v>
       </c>
-      <c r="B32" s="3" t="s">
-        <v>15</v>
+      <c r="B32" s="2" t="s">
+        <v>4</v>
       </c>
       <c r="C32" t="s">
         <v>11</v>
@@ -1474,21 +1499,21 @@
         <v>12</v>
       </c>
       <c r="E32">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F32">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G32">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" ht="15.75">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7">
       <c r="A33" t="s">
         <v>25</v>
       </c>
-      <c r="B33" s="3" t="s">
-        <v>15</v>
+      <c r="B33" s="2" t="s">
+        <v>4</v>
       </c>
       <c r="C33" t="s">
         <v>11</v>
@@ -1497,21 +1522,21 @@
         <v>13</v>
       </c>
       <c r="E33">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F33">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G33">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" ht="15.75">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7">
       <c r="A34" t="s">
         <v>25</v>
       </c>
-      <c r="B34" s="3" t="s">
-        <v>15</v>
+      <c r="B34" s="2" t="s">
+        <v>4</v>
       </c>
       <c r="C34" t="s">
         <v>11</v>
@@ -1520,21 +1545,21 @@
         <v>14</v>
       </c>
       <c r="E34">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F34">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G34">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" ht="15.75">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7">
       <c r="A35" t="s">
         <v>25</v>
       </c>
-      <c r="B35" s="3" t="s">
-        <v>15</v>
+      <c r="B35" s="2" t="s">
+        <v>4</v>
       </c>
       <c r="C35" t="s">
         <v>12</v>
@@ -1543,21 +1568,21 @@
         <v>11</v>
       </c>
       <c r="E35">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F35">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G35">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" ht="15.75">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7">
       <c r="A36" t="s">
         <v>25</v>
       </c>
-      <c r="B36" s="3" t="s">
-        <v>15</v>
+      <c r="B36" s="2" t="s">
+        <v>4</v>
       </c>
       <c r="C36" t="s">
         <v>12</v>
@@ -1566,21 +1591,21 @@
         <v>13</v>
       </c>
       <c r="E36">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F36">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G36">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" ht="15.75">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7">
       <c r="A37" t="s">
         <v>25</v>
       </c>
-      <c r="B37" s="3" t="s">
-        <v>15</v>
+      <c r="B37" s="2" t="s">
+        <v>4</v>
       </c>
       <c r="C37" t="s">
         <v>12</v>
@@ -1589,21 +1614,21 @@
         <v>14</v>
       </c>
       <c r="E37">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F37">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G37">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:7" ht="15.75">
       <c r="A38" t="s">
         <v>25</v>
       </c>
-      <c r="B38" s="4" t="s">
-        <v>16</v>
+      <c r="B38" s="3" t="s">
+        <v>15</v>
       </c>
       <c r="C38" t="s">
         <v>11</v>
@@ -1612,21 +1637,21 @@
         <v>12</v>
       </c>
       <c r="E38">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F38">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G38">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="15.75">
       <c r="A39" t="s">
         <v>25</v>
       </c>
-      <c r="B39" s="4" t="s">
-        <v>16</v>
+      <c r="B39" s="3" t="s">
+        <v>15</v>
       </c>
       <c r="C39" t="s">
         <v>11</v>
@@ -1635,21 +1660,21 @@
         <v>13</v>
       </c>
       <c r="E39">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F39">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G39">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="40" spans="1:7" ht="15.75">
       <c r="A40" t="s">
         <v>25</v>
       </c>
-      <c r="B40" s="4" t="s">
-        <v>16</v>
+      <c r="B40" s="3" t="s">
+        <v>15</v>
       </c>
       <c r="C40" t="s">
         <v>11</v>
@@ -1658,21 +1683,21 @@
         <v>14</v>
       </c>
       <c r="E40">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F40">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G40">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="41" spans="1:7" ht="15.75">
       <c r="A41" t="s">
         <v>25</v>
       </c>
-      <c r="B41" s="4" t="s">
-        <v>16</v>
+      <c r="B41" s="3" t="s">
+        <v>15</v>
       </c>
       <c r="C41" t="s">
         <v>12</v>
@@ -1681,21 +1706,21 @@
         <v>11</v>
       </c>
       <c r="E41">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F41">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G41">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="42" spans="1:7" ht="15.75">
       <c r="A42" t="s">
         <v>25</v>
       </c>
-      <c r="B42" s="4" t="s">
-        <v>16</v>
+      <c r="B42" s="3" t="s">
+        <v>15</v>
       </c>
       <c r="C42" t="s">
         <v>12</v>
@@ -1704,21 +1729,21 @@
         <v>13</v>
       </c>
       <c r="E42">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F42">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G42">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="43" spans="1:7" ht="15.75">
       <c r="A43" t="s">
         <v>25</v>
       </c>
-      <c r="B43" s="4" t="s">
-        <v>16</v>
+      <c r="B43" s="3" t="s">
+        <v>15</v>
       </c>
       <c r="C43" t="s">
         <v>12</v>
@@ -1727,13 +1752,13 @@
         <v>14</v>
       </c>
       <c r="E43">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F43">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G43">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="44" spans="1:7" ht="15.75">
@@ -1741,7 +1766,7 @@
         <v>25</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C44" t="s">
         <v>11</v>
@@ -1750,13 +1775,13 @@
         <v>12</v>
       </c>
       <c r="E44">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F44">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G44">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="45" spans="1:7" ht="15.75">
@@ -1764,7 +1789,7 @@
         <v>25</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C45" t="s">
         <v>11</v>
@@ -1773,13 +1798,13 @@
         <v>13</v>
       </c>
       <c r="E45">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F45">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G45">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="46" spans="1:7" ht="15.75">
@@ -1787,7 +1812,7 @@
         <v>25</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C46" t="s">
         <v>11</v>
@@ -1796,13 +1821,13 @@
         <v>14</v>
       </c>
       <c r="E46">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F46">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G46">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="47" spans="1:7" ht="15.75">
@@ -1810,7 +1835,7 @@
         <v>25</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C47" t="s">
         <v>12</v>
@@ -1819,13 +1844,13 @@
         <v>11</v>
       </c>
       <c r="E47">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F47">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G47">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="48" spans="1:7" ht="15.75">
@@ -1833,7 +1858,7 @@
         <v>25</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C48" t="s">
         <v>12</v>
@@ -1842,13 +1867,13 @@
         <v>13</v>
       </c>
       <c r="E48">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F48">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G48">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="49" spans="1:7" ht="15.75">
@@ -1856,7 +1881,7 @@
         <v>25</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C49" t="s">
         <v>12</v>
@@ -1865,12 +1890,150 @@
         <v>14</v>
       </c>
       <c r="E49">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F49">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G49">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" ht="15.75">
+      <c r="A50" t="s">
+        <v>25</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C50" t="s">
+        <v>11</v>
+      </c>
+      <c r="D50" t="s">
+        <v>12</v>
+      </c>
+      <c r="E50">
+        <v>4</v>
+      </c>
+      <c r="F50">
+        <v>4</v>
+      </c>
+      <c r="G50">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" ht="15.75">
+      <c r="A51" t="s">
+        <v>25</v>
+      </c>
+      <c r="B51" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C51" t="s">
+        <v>11</v>
+      </c>
+      <c r="D51" t="s">
+        <v>13</v>
+      </c>
+      <c r="E51">
+        <v>4</v>
+      </c>
+      <c r="F51">
+        <v>4</v>
+      </c>
+      <c r="G51">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" ht="15.75">
+      <c r="A52" t="s">
+        <v>25</v>
+      </c>
+      <c r="B52" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C52" t="s">
+        <v>11</v>
+      </c>
+      <c r="D52" t="s">
+        <v>14</v>
+      </c>
+      <c r="E52">
+        <v>4</v>
+      </c>
+      <c r="F52">
+        <v>4</v>
+      </c>
+      <c r="G52">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" ht="15.75">
+      <c r="A53" t="s">
+        <v>25</v>
+      </c>
+      <c r="B53" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C53" t="s">
+        <v>12</v>
+      </c>
+      <c r="D53" t="s">
+        <v>11</v>
+      </c>
+      <c r="E53">
+        <v>4</v>
+      </c>
+      <c r="F53">
+        <v>4</v>
+      </c>
+      <c r="G53">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" ht="15.75">
+      <c r="A54" t="s">
+        <v>25</v>
+      </c>
+      <c r="B54" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C54" t="s">
+        <v>12</v>
+      </c>
+      <c r="D54" t="s">
+        <v>13</v>
+      </c>
+      <c r="E54">
+        <v>4</v>
+      </c>
+      <c r="F54">
+        <v>4</v>
+      </c>
+      <c r="G54">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" ht="15.75">
+      <c r="A55" t="s">
+        <v>25</v>
+      </c>
+      <c r="B55" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C55" t="s">
+        <v>12</v>
+      </c>
+      <c r="D55" t="s">
+        <v>14</v>
+      </c>
+      <c r="E55">
+        <v>4</v>
+      </c>
+      <c r="F55">
+        <v>4</v>
+      </c>
+      <c r="G55">
         <v>4</v>
       </c>
     </row>

</xml_diff>